<commit_message>
update modules/kbase: add        1 mod        5 files
</commit_message>
<xml_diff>
--- a/starter/src/main/resources/static/excel/kbase_text.xlsx
+++ b/starter/src/main/resources/static/excel/kbase_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="31140" windowHeight="14360"/>
+    <workbookView windowWidth="27920" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="自动回复" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>分类(必填)</t>
   </si>
   <si>
-    <t>类型</t>
+    <t>标题</t>
   </si>
   <si>
     <t>文本内容</t>
@@ -41,13 +41,16 @@
     <t>分类1</t>
   </si>
   <si>
-    <t>TEXT</t>
+    <t>标题1</t>
   </si>
   <si>
     <t>内容1</t>
   </si>
   <si>
     <t>分类2</t>
+  </si>
+  <si>
+    <t>标题2</t>
   </si>
   <si>
     <t>内容2</t>
@@ -1052,7 +1055,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1089,10 +1092,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>